<commit_message>
Remove V47 validation scenario for now
</commit_message>
<xml_diff>
--- a/project_input_template/landbosse-expected-validation-data.xlsx
+++ b/project_input_template/landbosse-expected-validation-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/project_input_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C6B9C3-E773-BE4F-8203-0042A9698DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FF7B4B-A205-5C49-AEFD-94CF624E0689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27260" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27260" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs_by_module_type_operation" sheetId="1" r:id="rId1"/>
@@ -598,8 +598,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F249" sqref="F249"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="J21"/>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="J22"/>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="J28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="J29"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1745,14 +1745,14 @@
         <v>19</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" ref="G30:G55" si="0">H38</f>
+        <f t="shared" ref="G38:G55" si="0">H38</f>
         <v>0</v>
       </c>
       <c r="H38" s="2">
         <v>0</v>
       </c>
       <c r="I38" s="5">
-        <f t="shared" ref="I30:I55" si="1">H38/C38/1000</f>
+        <f t="shared" ref="I38:I55" si="1">H38/C38/1000</f>
         <v>0</v>
       </c>
       <c r="J38"/>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="J48"/>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -2085,23 +2085,21 @@
       <c r="E49" t="s">
         <v>13</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G49" s="2">
-        <f t="shared" si="0"/>
-        <v>7070.6972452158416</v>
-      </c>
-      <c r="H49" s="2">
-        <v>7070.6972452158416</v>
+      <c r="G49" s="5">
+        <v>6931.8389218436796</v>
+      </c>
+      <c r="H49" s="5">
+        <v>6931.8389218436796</v>
       </c>
       <c r="I49" s="5">
-        <f t="shared" si="1"/>
-        <v>4.7137981634772279</v>
+        <v>4.6212259478957902</v>
       </c>
       <c r="J49"/>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -2117,23 +2115,21 @@
       <c r="E50" t="s">
         <v>13</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G50" s="2">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-      <c r="H50" s="2">
-        <v>240</v>
+      <c r="G50" s="5">
+        <v>169.5</v>
+      </c>
+      <c r="H50" s="5">
+        <v>169.5</v>
       </c>
       <c r="I50" s="5">
-        <f t="shared" si="1"/>
-        <v>0.16</v>
+        <v>0.113</v>
       </c>
       <c r="J50"/>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -2149,23 +2145,21 @@
       <c r="E51" t="s">
         <v>13</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G51" s="2">
-        <f t="shared" si="0"/>
-        <v>35349.322678682678</v>
-      </c>
-      <c r="H51" s="2">
-        <v>35349.322678682678</v>
+      <c r="G51" s="5">
+        <v>49441.813382952401</v>
+      </c>
+      <c r="H51" s="5">
+        <v>49441.813382952401</v>
       </c>
       <c r="I51" s="5">
-        <f t="shared" si="1"/>
-        <v>23.566215119121786</v>
+        <v>32.961208921968201</v>
       </c>
       <c r="J51"/>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -2181,23 +2175,21 @@
       <c r="E52" t="s">
         <v>13</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G52" s="2">
-        <f t="shared" si="0"/>
-        <v>416000</v>
-      </c>
-      <c r="H52" s="2">
-        <v>416000</v>
+      <c r="G52" s="5">
+        <v>400956</v>
+      </c>
+      <c r="H52" s="5">
+        <v>400956</v>
       </c>
       <c r="I52" s="5">
-        <f t="shared" si="1"/>
-        <v>277.33333333333331</v>
+        <v>267.30399999999997</v>
       </c>
       <c r="J52"/>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -2213,23 +2205,21 @@
       <c r="E53" t="s">
         <v>13</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G53" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H53" s="2">
+      <c r="G53" s="5">
+        <v>0</v>
+      </c>
+      <c r="H53" s="5">
         <v>0</v>
       </c>
       <c r="I53" s="5">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -2245,18 +2235,16 @@
       <c r="E54" t="s">
         <v>13</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G54" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H54" s="2">
+      <c r="G54" s="5">
+        <v>0</v>
+      </c>
+      <c r="H54" s="5">
         <v>0</v>
       </c>
       <c r="I54" s="5">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J54" s="4"/>
@@ -2293,7 +2281,7 @@
       </c>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>39</v>
       </c>
@@ -2322,7 +2310,7 @@
         <v>2.0503571322296299</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>39</v>
       </c>
@@ -2351,7 +2339,7 @@
         <v>30.571233379056402</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>39</v>
       </c>
@@ -2380,7 +2368,7 @@
         <v>37.153541440447199</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>39</v>
       </c>
@@ -2574,14 +2562,14 @@
         <v>19</v>
       </c>
       <c r="G65" s="2">
-        <f t="shared" ref="G57:G108" si="2">H65/B65</f>
+        <f t="shared" ref="G65:G102" si="2">H65/B65</f>
         <v>0</v>
       </c>
       <c r="H65" s="2">
         <v>0</v>
       </c>
       <c r="I65" s="5">
-        <f t="shared" ref="I57:I108" si="3">G65/1500</f>
+        <f t="shared" ref="I65:I102" si="3">G65/1500</f>
         <v>0</v>
       </c>
     </row>
@@ -2887,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>39</v>
       </c>
@@ -2903,22 +2891,20 @@
       <c r="E76" t="s">
         <v>13</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G76" s="2">
-        <f t="shared" si="2"/>
-        <v>7070.6972452158416</v>
-      </c>
-      <c r="H76" s="2">
-        <v>35353.486226079207</v>
+      <c r="G76" s="5">
+        <v>6931.8389218436796</v>
+      </c>
+      <c r="H76" s="5">
+        <v>34659.194609218401</v>
       </c>
       <c r="I76" s="5">
-        <f t="shared" si="3"/>
-        <v>4.7137981634772279</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>4.6212259478957902</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>39</v>
       </c>
@@ -2934,22 +2920,20 @@
       <c r="E77" t="s">
         <v>13</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G77" s="2">
-        <f t="shared" si="2"/>
-        <v>321</v>
-      </c>
-      <c r="H77" s="2">
-        <v>1605</v>
+      <c r="G77" s="5">
+        <v>263.7</v>
+      </c>
+      <c r="H77" s="5">
+        <v>1318.5</v>
       </c>
       <c r="I77" s="5">
-        <f t="shared" si="3"/>
-        <v>0.214</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>0.17580000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -2965,22 +2949,20 @@
       <c r="E78" t="s">
         <v>13</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G78" s="2">
-        <f t="shared" si="2"/>
-        <v>36443.72267868268</v>
-      </c>
-      <c r="H78" s="2">
-        <v>182218.6133934134</v>
+      <c r="G78" s="5">
+        <v>51145.367149619</v>
+      </c>
+      <c r="H78" s="5">
+        <v>255726.83574809501</v>
       </c>
       <c r="I78" s="5">
-        <f t="shared" si="3"/>
-        <v>24.295815119121787</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>34.096911433079399</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>39</v>
       </c>
@@ -2996,22 +2978,20 @@
       <c r="E79" t="s">
         <v>13</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G79" s="2">
-        <f t="shared" si="2"/>
-        <v>83200</v>
-      </c>
-      <c r="H79" s="2">
-        <v>416000</v>
+      <c r="G79" s="5">
+        <v>80191.199999999997</v>
+      </c>
+      <c r="H79" s="5">
+        <v>400956</v>
       </c>
       <c r="I79" s="5">
-        <f t="shared" si="3"/>
-        <v>55.466666666666669</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>53.460799999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>39</v>
       </c>
@@ -3027,22 +3007,20 @@
       <c r="E80" t="s">
         <v>13</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G80" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H80" s="2">
+      <c r="G80" s="5">
+        <v>0</v>
+      </c>
+      <c r="H80" s="5">
         <v>0</v>
       </c>
       <c r="I80" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>39</v>
       </c>
@@ -3058,18 +3036,16 @@
       <c r="E81" t="s">
         <v>13</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G81" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H81" s="2">
+      <c r="G81" s="5">
+        <v>0</v>
+      </c>
+      <c r="H81" s="5">
         <v>0</v>
       </c>
       <c r="I81" s="5">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3104,7 +3080,7 @@
         <v>202.56666666666666</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>40</v>
       </c>
@@ -3134,7 +3110,7 @@
       </c>
       <c r="J83"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>40</v>
       </c>
@@ -3164,7 +3140,7 @@
       </c>
       <c r="J84"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>40</v>
       </c>
@@ -3194,7 +3170,7 @@
       </c>
       <c r="J85"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>40</v>
       </c>
@@ -3718,7 +3694,7 @@
       </c>
       <c r="J102"/>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>40</v>
       </c>
@@ -3734,23 +3710,21 @@
       <c r="E103" t="s">
         <v>13</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F103" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G103" s="2">
-        <f t="shared" si="2"/>
-        <v>7070.6972452158416</v>
-      </c>
-      <c r="H103" s="2">
-        <v>70706.972452158414</v>
+      <c r="G103" s="5">
+        <v>6931.8389218436796</v>
+      </c>
+      <c r="H103" s="5">
+        <v>69318.389218436801</v>
       </c>
       <c r="I103" s="5">
-        <f t="shared" si="3"/>
-        <v>4.7137981634772279</v>
+        <v>4.6212259478957902</v>
       </c>
       <c r="J103"/>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>40</v>
       </c>
@@ -3766,23 +3740,21 @@
       <c r="E104" t="s">
         <v>13</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F104" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G104" s="2">
-        <f t="shared" si="2"/>
-        <v>330</v>
-      </c>
-      <c r="H104" s="2">
-        <v>3300</v>
+      <c r="G104" s="5">
+        <v>293.85000000000002</v>
+      </c>
+      <c r="H104" s="5">
+        <v>2938.5</v>
       </c>
       <c r="I104" s="5">
-        <f t="shared" si="3"/>
-        <v>0.22</v>
+        <v>0.19589999999999999</v>
       </c>
       <c r="J104"/>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>40</v>
       </c>
@@ -3798,23 +3770,21 @@
       <c r="E105" t="s">
         <v>13</v>
       </c>
-      <c r="F105" t="s">
+      <c r="F105" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G105" s="2">
-        <f t="shared" si="2"/>
-        <v>36501.322678682678</v>
-      </c>
-      <c r="H105" s="2">
-        <v>365013.2267868268</v>
+      <c r="G105" s="5">
+        <v>51651.967149618999</v>
+      </c>
+      <c r="H105" s="5">
+        <v>516519.67149619001</v>
       </c>
       <c r="I105" s="5">
-        <f t="shared" si="3"/>
-        <v>24.334215119121787</v>
+        <v>34.434644766412703</v>
       </c>
       <c r="J105"/>
     </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>40</v>
       </c>
@@ -3830,23 +3800,21 @@
       <c r="E106" t="s">
         <v>13</v>
       </c>
-      <c r="F106" t="s">
+      <c r="F106" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G106" s="2">
-        <f t="shared" si="2"/>
-        <v>41600</v>
-      </c>
-      <c r="H106" s="2">
-        <v>416000</v>
+      <c r="G106" s="5">
+        <v>40095.599999999999</v>
+      </c>
+      <c r="H106" s="5">
+        <v>400956</v>
       </c>
       <c r="I106" s="5">
-        <f t="shared" si="3"/>
-        <v>27.733333333333334</v>
+        <v>26.730399999999999</v>
       </c>
       <c r="J106"/>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>40</v>
       </c>
@@ -3862,23 +3830,21 @@
       <c r="E107" t="s">
         <v>13</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F107" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G107" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H107" s="2">
+      <c r="G107" s="5">
+        <v>0</v>
+      </c>
+      <c r="H107" s="5">
         <v>0</v>
       </c>
       <c r="I107" s="5">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J107"/>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>40</v>
       </c>
@@ -3894,18 +3860,16 @@
       <c r="E108" t="s">
         <v>13</v>
       </c>
-      <c r="F108" t="s">
+      <c r="F108" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G108" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H108" s="2">
+      <c r="G108" s="5">
+        <v>0</v>
+      </c>
+      <c r="H108" s="5">
         <v>0</v>
       </c>
       <c r="I108" s="5">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J108"/>
@@ -4542,7 +4506,7 @@
       </c>
       <c r="J129"/>
     </row>
-    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>41</v>
       </c>
@@ -4561,18 +4525,18 @@
       <c r="F130" t="s">
         <v>15</v>
       </c>
-      <c r="G130">
+      <c r="G130" s="9">
         <v>7489.11492789153</v>
       </c>
-      <c r="H130">
+      <c r="H130" s="9">
         <v>748911.49278915301</v>
       </c>
-      <c r="I130" s="5">
+      <c r="I130" s="9">
         <v>4.9927432852610201</v>
       </c>
       <c r="J130"/>
     </row>
-    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>41</v>
       </c>
@@ -4591,18 +4555,18 @@
       <c r="F131" t="s">
         <v>20</v>
       </c>
-      <c r="G131">
+      <c r="G131" s="9">
         <v>288.255</v>
       </c>
-      <c r="H131">
+      <c r="H131" s="9">
         <v>28825.5</v>
       </c>
-      <c r="I131" s="5">
+      <c r="I131" s="9">
         <v>0.19217000000000001</v>
       </c>
       <c r="J131"/>
     </row>
-    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>41</v>
       </c>
@@ -4621,18 +4585,18 @@
       <c r="F132" t="s">
         <v>16</v>
       </c>
-      <c r="G132">
+      <c r="G132" s="9">
         <v>51346.538032382698</v>
       </c>
-      <c r="H132">
+      <c r="H132" s="9">
         <v>5134653.8032382699</v>
       </c>
-      <c r="I132" s="5">
+      <c r="I132" s="9">
         <v>34.231025354921798</v>
       </c>
       <c r="J132"/>
     </row>
-    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>41</v>
       </c>
@@ -4651,18 +4615,18 @@
       <c r="F133" t="s">
         <v>18</v>
       </c>
-      <c r="G133">
+      <c r="G133" s="9">
         <v>8993.1</v>
       </c>
-      <c r="H133">
+      <c r="H133" s="9">
         <v>899310</v>
       </c>
-      <c r="I133" s="5">
+      <c r="I133" s="9">
         <v>5.9954000000000001</v>
       </c>
       <c r="J133"/>
     </row>
-    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>41</v>
       </c>
@@ -4681,18 +4645,18 @@
       <c r="F134" t="s">
         <v>19</v>
       </c>
-      <c r="G134">
-        <v>0</v>
-      </c>
-      <c r="H134">
-        <v>0</v>
-      </c>
-      <c r="I134" s="5">
+      <c r="G134" s="9">
+        <v>0</v>
+      </c>
+      <c r="H134" s="9">
+        <v>0</v>
+      </c>
+      <c r="I134" s="9">
         <v>0</v>
       </c>
       <c r="J134"/>
     </row>
-    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>41</v>
       </c>
@@ -4711,13 +4675,13 @@
       <c r="F135" t="s">
         <v>17</v>
       </c>
-      <c r="G135">
-        <v>0</v>
-      </c>
-      <c r="H135">
-        <v>0</v>
-      </c>
-      <c r="I135" s="5">
+      <c r="G135" s="9">
+        <v>0</v>
+      </c>
+      <c r="H135" s="9">
+        <v>0</v>
+      </c>
+      <c r="I135" s="9">
         <v>0</v>
       </c>
       <c r="J135"/>
@@ -5532,7 +5496,7 @@
       </c>
       <c r="J162"/>
     </row>
-    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>42</v>
       </c>
@@ -5551,18 +5515,18 @@
       <c r="F163" t="s">
         <v>15</v>
       </c>
-      <c r="G163">
+      <c r="G163" s="9">
         <v>9442.9461961058605</v>
       </c>
-      <c r="H163">
+      <c r="H163" s="9">
         <v>566576.77176635095</v>
       </c>
-      <c r="I163" s="5">
+      <c r="I163" s="9">
         <v>3.7771784784423401</v>
       </c>
       <c r="J163"/>
     </row>
-    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>42</v>
       </c>
@@ -5581,18 +5545,18 @@
       <c r="F164" t="s">
         <v>20</v>
       </c>
-      <c r="G164">
+      <c r="G164" s="9">
         <v>304.5</v>
       </c>
-      <c r="H164">
+      <c r="H164" s="9">
         <v>18270</v>
       </c>
-      <c r="I164" s="5">
+      <c r="I164" s="9">
         <v>0.12180000000000001</v>
       </c>
       <c r="J164"/>
     </row>
-    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>42</v>
       </c>
@@ -5611,18 +5575,18 @@
       <c r="F165" t="s">
         <v>16</v>
       </c>
-      <c r="G165">
+      <c r="G165" s="9">
         <v>54137.465077806097</v>
       </c>
-      <c r="H165">
+      <c r="H165" s="9">
         <v>3248247.9046683698</v>
       </c>
-      <c r="I165" s="5">
+      <c r="I165" s="9">
         <v>21.654986031122402</v>
       </c>
       <c r="J165"/>
     </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>42</v>
       </c>
@@ -5641,18 +5605,18 @@
       <c r="F166" t="s">
         <v>18</v>
       </c>
-      <c r="G166">
+      <c r="G166" s="9">
         <v>10195.5666666666</v>
       </c>
-      <c r="H166">
+      <c r="H166" s="9">
         <v>611734</v>
       </c>
-      <c r="I166" s="5">
+      <c r="I166" s="9">
         <v>4.0782266666666596</v>
       </c>
       <c r="J166"/>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>42</v>
       </c>
@@ -5671,18 +5635,18 @@
       <c r="F167" t="s">
         <v>19</v>
       </c>
-      <c r="G167">
-        <v>0</v>
-      </c>
-      <c r="H167">
-        <v>0</v>
-      </c>
-      <c r="I167" s="5">
+      <c r="G167" s="9">
+        <v>0</v>
+      </c>
+      <c r="H167" s="9">
+        <v>0</v>
+      </c>
+      <c r="I167" s="9">
         <v>0</v>
       </c>
       <c r="J167"/>
     </row>
-    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>42</v>
       </c>
@@ -5701,13 +5665,13 @@
       <c r="F168" t="s">
         <v>17</v>
       </c>
-      <c r="G168">
-        <v>0</v>
-      </c>
-      <c r="H168">
-        <v>0</v>
-      </c>
-      <c r="I168" s="5">
+      <c r="G168" s="9">
+        <v>0</v>
+      </c>
+      <c r="H168" s="9">
+        <v>0</v>
+      </c>
+      <c r="I168" s="9">
         <v>0</v>
       </c>
       <c r="J168"/>
@@ -6522,7 +6486,7 @@
       </c>
       <c r="J195"/>
     </row>
-    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>43</v>
       </c>
@@ -6541,18 +6505,18 @@
       <c r="F196" t="s">
         <v>15</v>
       </c>
-      <c r="G196">
+      <c r="G196" s="9">
         <v>8523.1960817585805</v>
       </c>
-      <c r="H196">
+      <c r="H196" s="9">
         <v>238649.49028924</v>
       </c>
-      <c r="I196" s="5">
+      <c r="I196" s="9">
         <v>2.36755446715516</v>
       </c>
       <c r="J196"/>
     </row>
-    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>43</v>
       </c>
@@ -6571,18 +6535,18 @@
       <c r="F197" t="s">
         <v>20</v>
       </c>
-      <c r="G197">
+      <c r="G197" s="9">
         <v>345.375</v>
       </c>
-      <c r="H197">
+      <c r="H197" s="9">
         <v>9670.5</v>
       </c>
-      <c r="I197" s="5">
+      <c r="I197" s="9">
         <v>9.5937499999999995E-2</v>
       </c>
       <c r="J197"/>
     </row>
-    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>43</v>
       </c>
@@ -6601,18 +6565,18 @@
       <c r="F198" t="s">
         <v>16</v>
       </c>
-      <c r="G198">
+      <c r="G198" s="9">
         <v>73765.537350567</v>
       </c>
-      <c r="H198">
+      <c r="H198" s="9">
         <v>2065435.0458158699</v>
       </c>
-      <c r="I198" s="5">
+      <c r="I198" s="9">
         <v>20.490427041824098</v>
       </c>
       <c r="J198"/>
     </row>
-    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>43</v>
       </c>
@@ -6631,18 +6595,18 @@
       <c r="F199" t="s">
         <v>18</v>
       </c>
-      <c r="G199">
+      <c r="G199" s="9">
         <v>19227.6428571428</v>
       </c>
-      <c r="H199">
+      <c r="H199" s="9">
         <v>538374</v>
       </c>
-      <c r="I199" s="5">
+      <c r="I199" s="9">
         <v>5.3410119047619</v>
       </c>
       <c r="J199"/>
     </row>
-    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>43</v>
       </c>
@@ -6661,18 +6625,18 @@
       <c r="F200" t="s">
         <v>19</v>
       </c>
-      <c r="G200">
-        <v>0</v>
-      </c>
-      <c r="H200">
-        <v>0</v>
-      </c>
-      <c r="I200" s="5">
+      <c r="G200" s="9">
+        <v>0</v>
+      </c>
+      <c r="H200" s="9">
+        <v>0</v>
+      </c>
+      <c r="I200" s="9">
         <v>0</v>
       </c>
       <c r="J200"/>
     </row>
-    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>43</v>
       </c>
@@ -6691,13 +6655,13 @@
       <c r="F201" t="s">
         <v>17</v>
       </c>
-      <c r="G201">
-        <v>0</v>
-      </c>
-      <c r="H201">
-        <v>0</v>
-      </c>
-      <c r="I201" s="5">
+      <c r="G201" s="9">
+        <v>0</v>
+      </c>
+      <c r="H201" s="9">
+        <v>0</v>
+      </c>
+      <c r="I201" s="9">
         <v>0</v>
       </c>
       <c r="J201"/>
@@ -7498,7 +7462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>44</v>
       </c>
@@ -7517,17 +7481,17 @@
       <c r="F229" t="s">
         <v>15</v>
       </c>
-      <c r="G229">
+      <c r="G229" s="9">
         <v>15939.7749065055</v>
       </c>
-      <c r="H229">
+      <c r="H229" s="9">
         <v>446313.69738215499</v>
       </c>
-      <c r="I229" s="5">
+      <c r="I229" s="9">
         <v>4.4277152518070899</v>
       </c>
     </row>
-    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>44</v>
       </c>
@@ -7546,17 +7510,17 @@
       <c r="F230" t="s">
         <v>20</v>
       </c>
-      <c r="G230">
+      <c r="G230" s="9">
         <v>507.58928571428498</v>
       </c>
-      <c r="H230">
+      <c r="H230" s="9">
         <v>14212.5</v>
       </c>
-      <c r="I230" s="5">
+      <c r="I230" s="9">
         <v>0.140997023809523</v>
       </c>
     </row>
-    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>44</v>
       </c>
@@ -7575,17 +7539,17 @@
       <c r="F231" t="s">
         <v>16</v>
       </c>
-      <c r="G231">
+      <c r="G231" s="9">
         <v>85921.130323546604</v>
       </c>
-      <c r="H231">
+      <c r="H231" s="9">
         <v>2405791.6490592998</v>
       </c>
-      <c r="I231" s="5">
+      <c r="I231" s="9">
         <v>23.866980645429599</v>
       </c>
     </row>
-    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>44</v>
       </c>
@@ -7604,17 +7568,17 @@
       <c r="F232" t="s">
         <v>18</v>
       </c>
-      <c r="G232">
+      <c r="G232" s="9">
         <v>32118.214285714199</v>
       </c>
-      <c r="H232">
+      <c r="H232" s="9">
         <v>899310</v>
       </c>
-      <c r="I232" s="5">
+      <c r="I232" s="9">
         <v>8.9217261904761909</v>
       </c>
     </row>
-    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>44</v>
       </c>
@@ -7633,17 +7597,17 @@
       <c r="F233" t="s">
         <v>19</v>
       </c>
-      <c r="G233">
-        <v>0</v>
-      </c>
-      <c r="H233">
-        <v>0</v>
-      </c>
-      <c r="I233" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G233" s="9">
+        <v>0</v>
+      </c>
+      <c r="H233" s="9">
+        <v>0</v>
+      </c>
+      <c r="I233" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>44</v>
       </c>
@@ -7662,13 +7626,13 @@
       <c r="F234" t="s">
         <v>17</v>
       </c>
-      <c r="G234">
-        <v>0</v>
-      </c>
-      <c r="H234">
-        <v>0</v>
-      </c>
-      <c r="I234" s="5">
+      <c r="G234" s="9">
+        <v>0</v>
+      </c>
+      <c r="H234" s="9">
+        <v>0</v>
+      </c>
+      <c r="I234" s="9">
         <v>0</v>
       </c>
     </row>
@@ -7877,16 +7841,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I241" xr:uid="{74B3986E-2BCE-704E-B480-617FD308BB93}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="ge15_dist_01"/>
-        <filter val="ge15_dist_05"/>
-        <filter val="ge15_dist_10"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="FoundationCost"/>
+        <filter val="ErectionCost"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Update expected validation data to reflect 5% mobilization cost in Foundation develop branch has mob cost as 10% of total module cost (utility scale), but that is being changed to 5% instead
</commit_message>
<xml_diff>
--- a/project_input_template/landbosse-expected-validation-data.xlsx
+++ b/project_input_template/landbosse-expected-validation-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FF7B4B-A205-5C49-AEFD-94CF624E0689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847800AC-8570-0244-B7B4-5ABEB577BCCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27260" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,8 +598,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D198" sqref="D198"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K246" sqref="K246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -735,7 +735,7 @@
       </c>
       <c r="J4"/>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="J21"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="J22"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="J48"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="J49"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="J50"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="J51"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="J52"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -2219,7 +2219,7 @@
       </c>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>37.153541440447199</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>39</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>39</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>4.6212259478957902</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>39</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>0.17580000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>34.096911433079399</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>39</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>53.460799999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>39</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>39</v>
       </c>
@@ -3170,7 +3170,7 @@
       </c>
       <c r="J85"/>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>40</v>
       </c>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="J102"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>40</v>
       </c>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="J103"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>40</v>
       </c>
@@ -3754,7 +3754,7 @@
       </c>
       <c r="J104"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>40</v>
       </c>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="J105"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>40</v>
       </c>
@@ -3814,7 +3814,7 @@
       </c>
       <c r="J106"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>40</v>
       </c>
@@ -3844,7 +3844,7 @@
       </c>
       <c r="J107"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>40</v>
       </c>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="J112"/>
     </row>
-    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>41</v>
       </c>
@@ -4016,10 +4016,10 @@
         <v>18</v>
       </c>
       <c r="G113">
-        <v>9558.2447726232804</v>
+        <v>4779.1223863116402</v>
       </c>
       <c r="H113">
-        <v>955824.47726232803</v>
+        <v>477912.23863116401</v>
       </c>
       <c r="I113" s="5">
         <v>6.3721631817488502</v>
@@ -4506,7 +4506,7 @@
       </c>
       <c r="J129"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>41</v>
       </c>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="J130"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>41</v>
       </c>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="J131"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>41</v>
       </c>
@@ -4596,7 +4596,7 @@
       </c>
       <c r="J132"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>41</v>
       </c>
@@ -4626,7 +4626,7 @@
       </c>
       <c r="J133"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>41</v>
       </c>
@@ -4656,7 +4656,7 @@
       </c>
       <c r="J134"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>41</v>
       </c>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="J145"/>
     </row>
-    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>42</v>
       </c>
@@ -5006,10 +5006,10 @@
         <v>18</v>
       </c>
       <c r="G146">
-        <v>13767.1137355049</v>
+        <v>6883.5568677524498</v>
       </c>
       <c r="H146">
-        <v>826026.82413029601</v>
+        <v>413013.412065148</v>
       </c>
       <c r="I146" s="5">
         <v>5.5068454942019702</v>
@@ -5496,7 +5496,7 @@
       </c>
       <c r="J162"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>42</v>
       </c>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="J163"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>42</v>
       </c>
@@ -5556,7 +5556,7 @@
       </c>
       <c r="J164"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>42</v>
       </c>
@@ -5586,7 +5586,7 @@
       </c>
       <c r="J165"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>42</v>
       </c>
@@ -5616,7 +5616,7 @@
       </c>
       <c r="J166"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>42</v>
       </c>
@@ -5646,7 +5646,7 @@
       </c>
       <c r="J167"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>42</v>
       </c>
@@ -5976,7 +5976,7 @@
       </c>
       <c r="J178"/>
     </row>
-    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>43</v>
       </c>
@@ -5996,10 +5996,10 @@
         <v>18</v>
       </c>
       <c r="G179">
-        <v>22594.5166764401</v>
+        <v>11297.25833822005</v>
       </c>
       <c r="H179">
-        <v>632646.46694032406</v>
+        <v>316323.23347016203</v>
       </c>
       <c r="I179" s="5">
         <v>6.2762546323444903</v>
@@ -6486,7 +6486,7 @@
       </c>
       <c r="J195"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>43</v>
       </c>
@@ -6516,7 +6516,7 @@
       </c>
       <c r="J196"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>43</v>
       </c>
@@ -6546,7 +6546,7 @@
       </c>
       <c r="J197"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>43</v>
       </c>
@@ -6576,7 +6576,7 @@
       </c>
       <c r="J198"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>43</v>
       </c>
@@ -6606,7 +6606,7 @@
       </c>
       <c r="J199"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>43</v>
       </c>
@@ -6636,7 +6636,7 @@
       </c>
       <c r="J200"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>43</v>
       </c>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="J211"/>
     </row>
-    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>44</v>
       </c>
@@ -6986,10 +6986,10 @@
         <v>18</v>
       </c>
       <c r="G212">
-        <v>34095.177724386704</v>
+        <v>17047.588862193352</v>
       </c>
       <c r="H212">
-        <v>954664.97628282697</v>
+        <v>477332.48814141349</v>
       </c>
       <c r="I212" s="5">
         <v>9.4708827012185299</v>
@@ -7462,7 +7462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>44</v>
       </c>
@@ -7491,7 +7491,7 @@
         <v>4.4277152518070899</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>44</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>0.140997023809523</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>44</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>23.866980645429599</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>44</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>8.9217261904761909</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>44</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>44</v>
       </c>
@@ -7843,7 +7843,12 @@
   <autoFilter ref="A1:I241" xr:uid="{74B3986E-2BCE-704E-B480-617FD308BB93}">
     <filterColumn colId="3">
       <filters>
-        <filter val="ErectionCost"/>
+        <filter val="FoundationCost"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Mobilization"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Update expected validation results for utility management cost. THe mob cost multiplier was changed from 10% to 5% for utility projects, which impacts the total project cost.. And since management cost is a function of total project cost, the expected validation that was obtained for utility projects using results from develop branch, was failing. I updated the updated validation spreadsheet's management cost expected results only for branch issue_108_integrate_DW (and not yet for develop). The validation should now pass for management and foundation modules.
</commit_message>
<xml_diff>
--- a/project_input_template/landbosse-expected-validation-data.xlsx
+++ b/project_input_template/landbosse-expected-validation-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847800AC-8570-0244-B7B4-5ABEB577BCCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B5C786-07FF-1943-BDAA-3185A2792506}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27260" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,8 +598,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K246" sqref="K246"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K139" sqref="K139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -735,7 +735,7 @@
       </c>
       <c r="J4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2249,7 +2249,7 @@
       </c>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>37.153541440447199</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>39</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>39</v>
       </c>
@@ -3170,7 +3170,7 @@
       </c>
       <c r="J85"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>40</v>
       </c>
@@ -3874,7 +3874,7 @@
       </c>
       <c r="J108"/>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>40</v>
       </c>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="J112"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>41</v>
       </c>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="J135"/>
     </row>
-    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>41</v>
       </c>
@@ -4705,18 +4705,18 @@
       <c r="F136" t="s">
         <v>24</v>
       </c>
-      <c r="G136">
-        <v>1910.48209148397</v>
-      </c>
-      <c r="H136">
-        <v>191048.209148397</v>
-      </c>
-      <c r="I136" s="5">
-        <v>1.27365472765598</v>
+      <c r="G136" s="9">
+        <v>1883.71900612063</v>
+      </c>
+      <c r="H136" s="9">
+        <v>188371.90061206301</v>
+      </c>
+      <c r="I136" s="9">
+        <v>1.25581267074708</v>
       </c>
       <c r="J136"/>
     </row>
-    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>41</v>
       </c>
@@ -4735,18 +4735,18 @@
       <c r="F137" t="s">
         <v>22</v>
       </c>
-      <c r="G137">
-        <v>4102.8138499771203</v>
-      </c>
-      <c r="H137">
-        <v>410281.38499771198</v>
-      </c>
-      <c r="I137" s="5">
-        <v>2.7352092333180802</v>
+      <c r="G137" s="9">
+        <v>4007.2314022508899</v>
+      </c>
+      <c r="H137" s="9">
+        <v>400723.14022508898</v>
+      </c>
+      <c r="I137" s="9">
+        <v>2.6714876015005902</v>
       </c>
       <c r="J137"/>
     </row>
-    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>41</v>
       </c>
@@ -4765,18 +4765,18 @@
       <c r="F138" t="s">
         <v>26</v>
       </c>
-      <c r="G138">
+      <c r="G138" s="9">
         <v>18877.634920373399</v>
       </c>
-      <c r="H138">
+      <c r="H138" s="9">
         <v>1887763.4920373401</v>
       </c>
-      <c r="I138" s="5">
+      <c r="I138" s="9">
         <v>12.5850899469156</v>
       </c>
       <c r="J138"/>
     </row>
-    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>41</v>
       </c>
@@ -4795,18 +4795,18 @@
       <c r="F139" t="s">
         <v>21</v>
       </c>
-      <c r="G139">
-        <v>3411.5751633642399</v>
-      </c>
-      <c r="H139">
-        <v>341157.51633642399</v>
-      </c>
-      <c r="I139" s="5">
-        <v>2.2743834422428302</v>
+      <c r="G139" s="9">
+        <v>3363.7839395011201</v>
+      </c>
+      <c r="H139" s="9">
+        <v>336378.39395011298</v>
+      </c>
+      <c r="I139" s="9">
+        <v>2.2425226263340798</v>
       </c>
       <c r="J139"/>
     </row>
-    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>41</v>
       </c>
@@ -4825,18 +4825,18 @@
       <c r="F140" t="s">
         <v>25</v>
       </c>
-      <c r="G140">
-        <v>44418.708627002401</v>
-      </c>
-      <c r="H140">
-        <v>4441870.8627002398</v>
-      </c>
-      <c r="I140" s="5">
-        <v>29.612472418001602</v>
+      <c r="G140" s="9">
+        <v>43796.466892304699</v>
+      </c>
+      <c r="H140" s="9">
+        <v>4379646.68923047</v>
+      </c>
+      <c r="I140" s="9">
+        <v>29.1976445948698</v>
       </c>
       <c r="J140"/>
     </row>
-    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>41</v>
       </c>
@@ -4855,18 +4855,18 @@
       <c r="F141" t="s">
         <v>23</v>
       </c>
-      <c r="G141">
+      <c r="G141" s="9">
         <v>20713.25</v>
       </c>
-      <c r="H141">
+      <c r="H141" s="9">
         <v>2071325</v>
       </c>
-      <c r="I141" s="5">
+      <c r="I141" s="9">
         <v>13.8088333333333</v>
       </c>
       <c r="J141"/>
     </row>
-    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>41</v>
       </c>
@@ -4885,13 +4885,13 @@
       <c r="F142" t="s">
         <v>27</v>
       </c>
-      <c r="G142">
+      <c r="G142" s="9">
         <v>13067.4835</v>
       </c>
-      <c r="H142">
+      <c r="H142" s="9">
         <v>1306748.3500000001</v>
       </c>
-      <c r="I142" s="5">
+      <c r="I142" s="9">
         <v>8.71165566666666</v>
       </c>
       <c r="J142"/>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="J145"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>42</v>
       </c>
@@ -5676,7 +5676,7 @@
       </c>
       <c r="J168"/>
     </row>
-    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>42</v>
       </c>
@@ -5695,18 +5695,18 @@
       <c r="F169" t="s">
         <v>24</v>
       </c>
-      <c r="G169">
-        <v>2715.9001117631901</v>
-      </c>
-      <c r="H169">
-        <v>162954.00670579099</v>
-      </c>
-      <c r="I169" s="5">
-        <v>1.0863600447052699</v>
+      <c r="G169" s="9">
+        <v>2677.35219330378</v>
+      </c>
+      <c r="H169" s="9">
+        <v>160641.131598226</v>
+      </c>
+      <c r="I169" s="9">
+        <v>1.0709408773215101</v>
       </c>
       <c r="J169"/>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>42</v>
       </c>
@@ -5725,18 +5725,18 @@
       <c r="F170" t="s">
         <v>22</v>
       </c>
-      <c r="G170">
-        <v>6362.0983551444197</v>
-      </c>
-      <c r="H170">
-        <v>381725.90130866499</v>
-      </c>
-      <c r="I170" s="5">
-        <v>2.54483934205776</v>
+      <c r="G170" s="9">
+        <v>6224.4272177893599</v>
+      </c>
+      <c r="H170" s="9">
+        <v>373465.63306736201</v>
+      </c>
+      <c r="I170" s="9">
+        <v>2.48977088711574</v>
       </c>
       <c r="J170"/>
     </row>
-    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>42</v>
       </c>
@@ -5755,18 +5755,18 @@
       <c r="F171" t="s">
         <v>26</v>
       </c>
-      <c r="G171">
+      <c r="G171" s="9">
         <v>27236.217376004999</v>
       </c>
-      <c r="H171">
+      <c r="H171" s="9">
         <v>1634173.0425603001</v>
       </c>
-      <c r="I171" s="5">
+      <c r="I171" s="9">
         <v>10.894486950401999</v>
       </c>
       <c r="J171"/>
     </row>
-    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>42</v>
       </c>
@@ -5785,18 +5785,18 @@
       <c r="F172" t="s">
         <v>21</v>
       </c>
-      <c r="G172">
-        <v>4849.8216281485602</v>
-      </c>
-      <c r="H172">
-        <v>290989.29768891301</v>
-      </c>
-      <c r="I172" s="5">
-        <v>1.93992865125942</v>
+      <c r="G172" s="9">
+        <v>4780.9860594710399</v>
+      </c>
+      <c r="H172" s="9">
+        <v>286859.16356826201</v>
+      </c>
+      <c r="I172" s="9">
+        <v>1.9123944237884101</v>
       </c>
       <c r="J172"/>
     </row>
-    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>42</v>
       </c>
@@ -5815,18 +5815,18 @@
       <c r="F173" t="s">
         <v>25</v>
       </c>
-      <c r="G173">
-        <v>63144.677598494301</v>
-      </c>
-      <c r="H173">
-        <v>3788680.65590965</v>
-      </c>
-      <c r="I173" s="5">
-        <v>25.257871039397699</v>
+      <c r="G173" s="9">
+        <v>62248.438494312897</v>
+      </c>
+      <c r="H173" s="9">
+        <v>3734906.30965877</v>
+      </c>
+      <c r="I173" s="9">
+        <v>24.899375397725098</v>
       </c>
       <c r="J173"/>
     </row>
-    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>42</v>
       </c>
@@ -5845,18 +5845,18 @@
       <c r="F174" t="s">
         <v>23</v>
       </c>
-      <c r="G174">
+      <c r="G174" s="9">
         <v>29169.75</v>
       </c>
-      <c r="H174">
+      <c r="H174" s="9">
         <v>1750185</v>
       </c>
-      <c r="I174" s="5">
+      <c r="I174" s="9">
         <v>11.667899999999999</v>
       </c>
       <c r="J174"/>
     </row>
-    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>42</v>
       </c>
@@ -5875,13 +5875,13 @@
       <c r="F175" t="s">
         <v>27</v>
       </c>
-      <c r="G175">
+      <c r="G175" s="9">
         <v>18172.713366666601</v>
       </c>
-      <c r="H175">
+      <c r="H175" s="9">
         <v>1090362.8019999999</v>
       </c>
-      <c r="I175" s="5">
+      <c r="I175" s="9">
         <v>7.2690853466666603</v>
       </c>
       <c r="J175"/>
@@ -5976,7 +5976,7 @@
       </c>
       <c r="J178"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>43</v>
       </c>
@@ -6666,7 +6666,7 @@
       </c>
       <c r="J201"/>
     </row>
-    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>43</v>
       </c>
@@ -6685,18 +6685,18 @@
       <c r="F202" t="s">
         <v>24</v>
       </c>
-      <c r="G202">
-        <v>4547.2666397718403</v>
-      </c>
-      <c r="H202">
-        <v>127323.465913611</v>
-      </c>
-      <c r="I202" s="5">
-        <v>1.2631296221588399</v>
+      <c r="G202" s="9">
+        <v>4484.0019930777999</v>
+      </c>
+      <c r="H202" s="9">
+        <v>125552.055806178</v>
+      </c>
+      <c r="I202" s="9">
+        <v>1.2455561091882801</v>
       </c>
       <c r="J202"/>
     </row>
-    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>43</v>
       </c>
@@ -6715,18 +6715,18 @@
       <c r="F203" t="s">
         <v>22</v>
       </c>
-      <c r="G203">
-        <v>12113.650811673901</v>
-      </c>
-      <c r="H203">
-        <v>339182.22272687103</v>
-      </c>
-      <c r="I203" s="5">
-        <v>3.36490300324277</v>
+      <c r="G203" s="9">
+        <v>11887.7056449095</v>
+      </c>
+      <c r="H203" s="9">
+        <v>332855.75805746799</v>
+      </c>
+      <c r="I203" s="9">
+        <v>3.3021404569193198</v>
       </c>
       <c r="J203"/>
     </row>
-    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>43</v>
       </c>
@@ -6745,18 +6745,18 @@
       <c r="F204" t="s">
         <v>26</v>
       </c>
-      <c r="G204">
+      <c r="G204" s="9">
         <v>55117.699983321399</v>
       </c>
-      <c r="H204">
+      <c r="H204" s="9">
         <v>1543295.59953299</v>
       </c>
-      <c r="I204" s="5">
+      <c r="I204" s="9">
         <v>15.310472217589201</v>
       </c>
       <c r="J204"/>
     </row>
-    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>43</v>
       </c>
@@ -6775,18 +6775,18 @@
       <c r="F205" t="s">
         <v>21</v>
       </c>
-      <c r="G205">
-        <v>8120.1189995925697</v>
-      </c>
-      <c r="H205">
-        <v>227363.33198859199</v>
-      </c>
-      <c r="I205" s="5">
-        <v>2.25558861099793</v>
+      <c r="G205" s="9">
+        <v>8007.1464162103703</v>
+      </c>
+      <c r="H205" s="9">
+        <v>224200.09965389001</v>
+      </c>
+      <c r="I205" s="9">
+        <v>2.2242073378362099</v>
       </c>
       <c r="J205"/>
     </row>
-    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>43</v>
       </c>
@@ -6805,18 +6805,18 @@
       <c r="F206" t="s">
         <v>25</v>
       </c>
-      <c r="G206">
-        <v>105723.949374695</v>
-      </c>
-      <c r="H206">
-        <v>2960270.5824914598</v>
-      </c>
-      <c r="I206" s="5">
-        <v>29.367763715193099</v>
+      <c r="G206" s="9">
+        <v>104253.046339059</v>
+      </c>
+      <c r="H206" s="9">
+        <v>2919085.2974936501</v>
+      </c>
+      <c r="I206" s="9">
+        <v>28.959179538627499</v>
       </c>
       <c r="J206"/>
     </row>
-    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>43</v>
       </c>
@@ -6835,18 +6835,18 @@
       <c r="F207" t="s">
         <v>23</v>
       </c>
-      <c r="G207">
+      <c r="G207" s="9">
         <v>52491.1785714285</v>
       </c>
-      <c r="H207">
+      <c r="H207" s="9">
         <v>1469753</v>
       </c>
-      <c r="I207" s="5">
+      <c r="I207" s="9">
         <v>14.5808829365079</v>
       </c>
       <c r="J207"/>
     </row>
-    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>43</v>
       </c>
@@ -6865,13 +6865,13 @@
       <c r="F208" t="s">
         <v>27</v>
       </c>
-      <c r="G208">
+      <c r="G208" s="9">
         <v>30052.964285714199</v>
       </c>
-      <c r="H208">
+      <c r="H208" s="9">
         <v>841483</v>
       </c>
-      <c r="I208" s="5">
+      <c r="I208" s="9">
         <v>8.3480456349206307</v>
       </c>
       <c r="J208"/>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="J211"/>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>44</v>
       </c>
@@ -7636,7 +7636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>44</v>
       </c>
@@ -7655,17 +7655,17 @@
       <c r="F235" t="s">
         <v>24</v>
       </c>
-      <c r="G235">
-        <v>5438.4071223926103</v>
-      </c>
-      <c r="H235">
-        <v>152275.39942699301</v>
-      </c>
-      <c r="I235" s="5">
-        <v>1.5106686451090601</v>
-      </c>
-    </row>
-    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G235" s="9">
+        <v>5342.9406247643301</v>
+      </c>
+      <c r="H235" s="9">
+        <v>149602.33749340099</v>
+      </c>
+      <c r="I235" s="9">
+        <v>1.4841501735456399</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>44</v>
       </c>
@@ -7684,17 +7684,17 @@
       <c r="F236" t="s">
         <v>22</v>
       </c>
-      <c r="G236">
-        <v>14643.796242222201</v>
-      </c>
-      <c r="H236">
-        <v>410026.29478222202</v>
-      </c>
-      <c r="I236" s="5">
-        <v>4.0677211783950602</v>
-      </c>
-    </row>
-    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G236" s="9">
+        <v>14302.8444649783</v>
+      </c>
+      <c r="H236" s="9">
+        <v>400479.64501939301</v>
+      </c>
+      <c r="I236" s="9">
+        <v>3.9730123513828701</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>44</v>
       </c>
@@ -7713,17 +7713,17 @@
       <c r="F237" t="s">
         <v>26</v>
       </c>
-      <c r="G237">
+      <c r="G237" s="9">
         <v>55117.699983321399</v>
       </c>
-      <c r="H237">
+      <c r="H237" s="9">
         <v>1543295.59953299</v>
       </c>
-      <c r="I237" s="5">
+      <c r="I237" s="9">
         <v>15.310472217589201</v>
       </c>
     </row>
-    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>44</v>
       </c>
@@ -7742,17 +7742,17 @@
       <c r="F238" t="s">
         <v>21</v>
       </c>
-      <c r="G238">
-        <v>9711.4412899868094</v>
-      </c>
-      <c r="H238">
-        <v>271920.35611962999</v>
-      </c>
-      <c r="I238" s="5">
-        <v>2.6976225805518901</v>
-      </c>
-    </row>
-    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G238" s="9">
+        <v>9540.9654013648797</v>
+      </c>
+      <c r="H238" s="9">
+        <v>267147.03123821598</v>
+      </c>
+      <c r="I238" s="9">
+        <v>2.6502681670457999</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>44</v>
       </c>
@@ -7771,17 +7771,17 @@
       <c r="F239" t="s">
         <v>25</v>
       </c>
-      <c r="G239">
-        <v>126442.965595628</v>
-      </c>
-      <c r="H239">
-        <v>3540403.0366775901</v>
-      </c>
-      <c r="I239" s="5">
-        <v>35.123045998785599</v>
-      </c>
-    </row>
-    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G239" s="9">
+        <v>124223.36952577</v>
+      </c>
+      <c r="H239" s="9">
+        <v>3478254.3467215798</v>
+      </c>
+      <c r="I239" s="9">
+        <v>34.506491534936302</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>44</v>
       </c>
@@ -7800,17 +7800,17 @@
       <c r="F240" t="s">
         <v>23</v>
       </c>
-      <c r="G240">
+      <c r="G240" s="9">
         <v>60048.321428571398</v>
       </c>
-      <c r="H240">
+      <c r="H240" s="9">
         <v>1681353</v>
       </c>
-      <c r="I240" s="5">
+      <c r="I240" s="9">
         <v>16.6800892857142</v>
       </c>
     </row>
-    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>44</v>
       </c>
@@ -7829,13 +7829,13 @@
       <c r="F241" t="s">
         <v>27</v>
       </c>
-      <c r="G241">
+      <c r="G241" s="9">
         <v>30052.964285714199</v>
       </c>
-      <c r="H241">
+      <c r="H241" s="9">
         <v>841483</v>
       </c>
-      <c r="I241" s="5">
+      <c r="I241" s="9">
         <v>8.3480456349206307</v>
       </c>
     </row>
@@ -7843,12 +7843,7 @@
   <autoFilter ref="A1:I241" xr:uid="{74B3986E-2BCE-704E-B480-617FD308BB93}">
     <filterColumn colId="3">
       <filters>
-        <filter val="FoundationCost"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Mobilization"/>
+        <filter val="ManagementCost"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Update gridconnection's validation data for DW. equation for tower_to_point_of_interconnection_usd_per_kw was updated, however the expected validation results for GridConnection module were obtained from the older, outdated equation for tower_to_point_of_interconnection_usd_per_kw. This has been fixed in this commit
</commit_message>
<xml_diff>
--- a/project_input_template/landbosse-expected-validation-data.xlsx
+++ b/project_input_template/landbosse-expected-validation-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B5C786-07FF-1943-BDAA-3185A2792506}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6043AD6-A56F-954E-B0FD-CA806B7C9815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27260" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,7 +599,7 @@
   <dimension ref="A1:J241"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K139" sqref="K139"/>
+      <selection activeCell="H250" sqref="H250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -945,7 +945,7 @@
       </c>
       <c r="J11"/>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="J38"/>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1776,16 +1776,14 @@
       <c r="F39" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="2">
-        <f t="shared" si="0"/>
-        <v>371334.19536712352</v>
-      </c>
-      <c r="H39" s="2">
-        <v>371334.19536712352</v>
-      </c>
-      <c r="I39" s="5">
-        <f t="shared" si="1"/>
-        <v>247.55613024474903</v>
+      <c r="G39" s="9">
+        <v>356384.85580801498</v>
+      </c>
+      <c r="H39" s="9">
+        <v>356384.85580801498</v>
+      </c>
+      <c r="I39" s="9">
+        <v>237.58990387201001</v>
       </c>
       <c r="J39"/>
     </row>
@@ -2249,7 +2247,7 @@
       </c>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -2573,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>39</v>
       </c>
@@ -2592,16 +2590,14 @@
       <c r="F66" t="s">
         <v>19</v>
       </c>
-      <c r="G66" s="2">
-        <f t="shared" si="2"/>
-        <v>371334.19536712341</v>
-      </c>
-      <c r="H66" s="2">
-        <v>1856670.9768356171</v>
-      </c>
-      <c r="I66" s="5">
-        <f t="shared" si="3"/>
-        <v>247.55613024474894</v>
+      <c r="G66" s="9">
+        <v>230037.90286025999</v>
+      </c>
+      <c r="H66" s="9">
+        <v>1150189.5143013</v>
+      </c>
+      <c r="I66" s="9">
+        <v>153.35860190683999</v>
       </c>
     </row>
     <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -3049,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>39</v>
       </c>
@@ -3382,7 +3378,7 @@
       </c>
       <c r="J92"/>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>40</v>
       </c>
@@ -3401,16 +3397,14 @@
       <c r="F93" t="s">
         <v>19</v>
       </c>
-      <c r="G93" s="2">
-        <f t="shared" si="2"/>
-        <v>371334.19536712352</v>
-      </c>
-      <c r="H93" s="2">
-        <v>3713341.9536712351</v>
-      </c>
-      <c r="I93" s="5">
-        <f t="shared" si="3"/>
-        <v>247.55613024474903</v>
+      <c r="G93" s="9">
+        <v>190510.64214379399</v>
+      </c>
+      <c r="H93" s="9">
+        <v>1905106.4214379401</v>
+      </c>
+      <c r="I93" s="9">
+        <v>127.00709476252899</v>
       </c>
       <c r="J93"/>
     </row>
@@ -3874,7 +3868,7 @@
       </c>
       <c r="J108"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>40</v>
       </c>
@@ -4206,7 +4200,7 @@
       </c>
       <c r="J119"/>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>41</v>
       </c>
@@ -4686,7 +4680,7 @@
       </c>
       <c r="J135"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>41</v>
       </c>
@@ -4716,7 +4710,7 @@
       </c>
       <c r="J136"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>41</v>
       </c>
@@ -4746,7 +4740,7 @@
       </c>
       <c r="J137"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>41</v>
       </c>
@@ -4776,7 +4770,7 @@
       </c>
       <c r="J138"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>41</v>
       </c>
@@ -4806,7 +4800,7 @@
       </c>
       <c r="J139"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>41</v>
       </c>
@@ -4836,7 +4830,7 @@
       </c>
       <c r="J140"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>41</v>
       </c>
@@ -4866,7 +4860,7 @@
       </c>
       <c r="J141"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>41</v>
       </c>
@@ -5196,7 +5190,7 @@
       </c>
       <c r="J152"/>
     </row>
-    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>42</v>
       </c>
@@ -5676,7 +5670,7 @@
       </c>
       <c r="J168"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>42</v>
       </c>
@@ -5706,7 +5700,7 @@
       </c>
       <c r="J169"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>42</v>
       </c>
@@ -5736,7 +5730,7 @@
       </c>
       <c r="J170"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>42</v>
       </c>
@@ -5766,7 +5760,7 @@
       </c>
       <c r="J171"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>42</v>
       </c>
@@ -5796,7 +5790,7 @@
       </c>
       <c r="J172"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>42</v>
       </c>
@@ -5826,7 +5820,7 @@
       </c>
       <c r="J173"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>42</v>
       </c>
@@ -5856,7 +5850,7 @@
       </c>
       <c r="J174"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>42</v>
       </c>
@@ -6186,7 +6180,7 @@
       </c>
       <c r="J185"/>
     </row>
-    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>43</v>
       </c>
@@ -6666,7 +6660,7 @@
       </c>
       <c r="J201"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>43</v>
       </c>
@@ -6696,7 +6690,7 @@
       </c>
       <c r="J202"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>43</v>
       </c>
@@ -6726,7 +6720,7 @@
       </c>
       <c r="J203"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>43</v>
       </c>
@@ -6756,7 +6750,7 @@
       </c>
       <c r="J204"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>43</v>
       </c>
@@ -6786,7 +6780,7 @@
       </c>
       <c r="J205"/>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>43</v>
       </c>
@@ -6816,7 +6810,7 @@
       </c>
       <c r="J206"/>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>43</v>
       </c>
@@ -6846,7 +6840,7 @@
       </c>
       <c r="J207"/>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>43</v>
       </c>
@@ -7172,7 +7166,7 @@
         <v>42.427747795912303</v>
       </c>
     </row>
-    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>44</v>
       </c>
@@ -7636,7 +7630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>44</v>
       </c>
@@ -7665,7 +7659,7 @@
         <v>1.4841501735456399</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>44</v>
       </c>
@@ -7694,7 +7688,7 @@
         <v>3.9730123513828701</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>44</v>
       </c>
@@ -7723,7 +7717,7 @@
         <v>15.310472217589201</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>44</v>
       </c>
@@ -7752,7 +7746,7 @@
         <v>2.6502681670457999</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>44</v>
       </c>
@@ -7781,7 +7775,7 @@
         <v>34.506491534936302</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>44</v>
       </c>
@@ -7810,7 +7804,7 @@
         <v>16.6800892857142</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>44</v>
       </c>
@@ -7843,7 +7837,7 @@
   <autoFilter ref="A1:I241" xr:uid="{74B3986E-2BCE-704E-B480-617FD308BB93}">
     <filterColumn colId="3">
       <filters>
-        <filter val="ManagementCost"/>
+        <filter val="GridConnectionCost"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
update landbosse-expected-validation-data.xlsx to V2. V2 of landbosse-expected-validation-data can be found in https://nrel.app.box.com/folder/111662093575. Running develop branch with this new, updated landbosse-expected-validation-data.xlsx data will make the validation fail because develop branch still has foundation module's mobilization cost at 10% of project_value_USD. And accordingly, this discrepancy in project_value_USD will cause management cost module to fail validation because management module is a function of project_value_USD. 
But this will automatically be fixed when branch issue_108_integrate_DW gets merged into develop.
</commit_message>
<xml_diff>
--- a/project_input_template/landbosse-expected-validation-data.xlsx
+++ b/project_input_template/landbosse-expected-validation-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/project_input_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FF7B4B-A205-5C49-AEFD-94CF624E0689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6043AD6-A56F-954E-B0FD-CA806B7C9815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27260" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,8 +598,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D198" sqref="D198"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H250" sqref="H250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -945,7 +945,7 @@
       </c>
       <c r="J11"/>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="J21"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="J22"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="J38"/>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1776,16 +1776,14 @@
       <c r="F39" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="2">
-        <f t="shared" si="0"/>
-        <v>371334.19536712352</v>
-      </c>
-      <c r="H39" s="2">
-        <v>371334.19536712352</v>
-      </c>
-      <c r="I39" s="5">
-        <f t="shared" si="1"/>
-        <v>247.55613024474903</v>
+      <c r="G39" s="9">
+        <v>356384.85580801498</v>
+      </c>
+      <c r="H39" s="9">
+        <v>356384.85580801498</v>
+      </c>
+      <c r="I39" s="9">
+        <v>237.58990387201001</v>
       </c>
       <c r="J39"/>
     </row>
@@ -2069,7 +2067,7 @@
       </c>
       <c r="J48"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -2099,7 +2097,7 @@
       </c>
       <c r="J49"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -2129,7 +2127,7 @@
       </c>
       <c r="J50"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -2159,7 +2157,7 @@
       </c>
       <c r="J51"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -2189,7 +2187,7 @@
       </c>
       <c r="J52"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -2219,7 +2217,7 @@
       </c>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -2573,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>39</v>
       </c>
@@ -2592,16 +2590,14 @@
       <c r="F66" t="s">
         <v>19</v>
       </c>
-      <c r="G66" s="2">
-        <f t="shared" si="2"/>
-        <v>371334.19536712341</v>
-      </c>
-      <c r="H66" s="2">
-        <v>1856670.9768356171</v>
-      </c>
-      <c r="I66" s="5">
-        <f t="shared" si="3"/>
-        <v>247.55613024474894</v>
+      <c r="G66" s="9">
+        <v>230037.90286025999</v>
+      </c>
+      <c r="H66" s="9">
+        <v>1150189.5143013</v>
+      </c>
+      <c r="I66" s="9">
+        <v>153.35860190683999</v>
       </c>
     </row>
     <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -2875,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>39</v>
       </c>
@@ -2904,7 +2900,7 @@
         <v>4.6212259478957902</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>39</v>
       </c>
@@ -2933,7 +2929,7 @@
         <v>0.17580000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -2962,7 +2958,7 @@
         <v>34.096911433079399</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>39</v>
       </c>
@@ -2991,7 +2987,7 @@
         <v>53.460799999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>39</v>
       </c>
@@ -3020,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>39</v>
       </c>
@@ -3382,7 +3378,7 @@
       </c>
       <c r="J92"/>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>40</v>
       </c>
@@ -3401,16 +3397,14 @@
       <c r="F93" t="s">
         <v>19</v>
       </c>
-      <c r="G93" s="2">
-        <f t="shared" si="2"/>
-        <v>371334.19536712352</v>
-      </c>
-      <c r="H93" s="2">
-        <v>3713341.9536712351</v>
-      </c>
-      <c r="I93" s="5">
-        <f t="shared" si="3"/>
-        <v>247.55613024474903</v>
+      <c r="G93" s="9">
+        <v>190510.64214379399</v>
+      </c>
+      <c r="H93" s="9">
+        <v>1905106.4214379401</v>
+      </c>
+      <c r="I93" s="9">
+        <v>127.00709476252899</v>
       </c>
       <c r="J93"/>
     </row>
@@ -3694,7 +3688,7 @@
       </c>
       <c r="J102"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>40</v>
       </c>
@@ -3724,7 +3718,7 @@
       </c>
       <c r="J103"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>40</v>
       </c>
@@ -3754,7 +3748,7 @@
       </c>
       <c r="J104"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>40</v>
       </c>
@@ -3784,7 +3778,7 @@
       </c>
       <c r="J105"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>40</v>
       </c>
@@ -3814,7 +3808,7 @@
       </c>
       <c r="J106"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>40</v>
       </c>
@@ -3844,7 +3838,7 @@
       </c>
       <c r="J107"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>40</v>
       </c>
@@ -4016,10 +4010,10 @@
         <v>18</v>
       </c>
       <c r="G113">
-        <v>9558.2447726232804</v>
+        <v>4779.1223863116402</v>
       </c>
       <c r="H113">
-        <v>955824.47726232803</v>
+        <v>477912.23863116401</v>
       </c>
       <c r="I113" s="5">
         <v>6.3721631817488502</v>
@@ -4206,7 +4200,7 @@
       </c>
       <c r="J119"/>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>41</v>
       </c>
@@ -4506,7 +4500,7 @@
       </c>
       <c r="J129"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>41</v>
       </c>
@@ -4536,7 +4530,7 @@
       </c>
       <c r="J130"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>41</v>
       </c>
@@ -4566,7 +4560,7 @@
       </c>
       <c r="J131"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>41</v>
       </c>
@@ -4596,7 +4590,7 @@
       </c>
       <c r="J132"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>41</v>
       </c>
@@ -4626,7 +4620,7 @@
       </c>
       <c r="J133"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>41</v>
       </c>
@@ -4656,7 +4650,7 @@
       </c>
       <c r="J134"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>41</v>
       </c>
@@ -4705,14 +4699,14 @@
       <c r="F136" t="s">
         <v>24</v>
       </c>
-      <c r="G136">
-        <v>1910.48209148397</v>
-      </c>
-      <c r="H136">
-        <v>191048.209148397</v>
-      </c>
-      <c r="I136" s="5">
-        <v>1.27365472765598</v>
+      <c r="G136" s="9">
+        <v>1883.71900612063</v>
+      </c>
+      <c r="H136" s="9">
+        <v>188371.90061206301</v>
+      </c>
+      <c r="I136" s="9">
+        <v>1.25581267074708</v>
       </c>
       <c r="J136"/>
     </row>
@@ -4735,14 +4729,14 @@
       <c r="F137" t="s">
         <v>22</v>
       </c>
-      <c r="G137">
-        <v>4102.8138499771203</v>
-      </c>
-      <c r="H137">
-        <v>410281.38499771198</v>
-      </c>
-      <c r="I137" s="5">
-        <v>2.7352092333180802</v>
+      <c r="G137" s="9">
+        <v>4007.2314022508899</v>
+      </c>
+      <c r="H137" s="9">
+        <v>400723.14022508898</v>
+      </c>
+      <c r="I137" s="9">
+        <v>2.6714876015005902</v>
       </c>
       <c r="J137"/>
     </row>
@@ -4765,13 +4759,13 @@
       <c r="F138" t="s">
         <v>26</v>
       </c>
-      <c r="G138">
+      <c r="G138" s="9">
         <v>18877.634920373399</v>
       </c>
-      <c r="H138">
+      <c r="H138" s="9">
         <v>1887763.4920373401</v>
       </c>
-      <c r="I138" s="5">
+      <c r="I138" s="9">
         <v>12.5850899469156</v>
       </c>
       <c r="J138"/>
@@ -4795,14 +4789,14 @@
       <c r="F139" t="s">
         <v>21</v>
       </c>
-      <c r="G139">
-        <v>3411.5751633642399</v>
-      </c>
-      <c r="H139">
-        <v>341157.51633642399</v>
-      </c>
-      <c r="I139" s="5">
-        <v>2.2743834422428302</v>
+      <c r="G139" s="9">
+        <v>3363.7839395011201</v>
+      </c>
+      <c r="H139" s="9">
+        <v>336378.39395011298</v>
+      </c>
+      <c r="I139" s="9">
+        <v>2.2425226263340798</v>
       </c>
       <c r="J139"/>
     </row>
@@ -4825,14 +4819,14 @@
       <c r="F140" t="s">
         <v>25</v>
       </c>
-      <c r="G140">
-        <v>44418.708627002401</v>
-      </c>
-      <c r="H140">
-        <v>4441870.8627002398</v>
-      </c>
-      <c r="I140" s="5">
-        <v>29.612472418001602</v>
+      <c r="G140" s="9">
+        <v>43796.466892304699</v>
+      </c>
+      <c r="H140" s="9">
+        <v>4379646.68923047</v>
+      </c>
+      <c r="I140" s="9">
+        <v>29.1976445948698</v>
       </c>
       <c r="J140"/>
     </row>
@@ -4855,13 +4849,13 @@
       <c r="F141" t="s">
         <v>23</v>
       </c>
-      <c r="G141">
+      <c r="G141" s="9">
         <v>20713.25</v>
       </c>
-      <c r="H141">
+      <c r="H141" s="9">
         <v>2071325</v>
       </c>
-      <c r="I141" s="5">
+      <c r="I141" s="9">
         <v>13.8088333333333</v>
       </c>
       <c r="J141"/>
@@ -4885,13 +4879,13 @@
       <c r="F142" t="s">
         <v>27</v>
       </c>
-      <c r="G142">
+      <c r="G142" s="9">
         <v>13067.4835</v>
       </c>
-      <c r="H142">
+      <c r="H142" s="9">
         <v>1306748.3500000001</v>
       </c>
-      <c r="I142" s="5">
+      <c r="I142" s="9">
         <v>8.71165566666666</v>
       </c>
       <c r="J142"/>
@@ -5006,10 +5000,10 @@
         <v>18</v>
       </c>
       <c r="G146">
-        <v>13767.1137355049</v>
+        <v>6883.5568677524498</v>
       </c>
       <c r="H146">
-        <v>826026.82413029601</v>
+        <v>413013.412065148</v>
       </c>
       <c r="I146" s="5">
         <v>5.5068454942019702</v>
@@ -5196,7 +5190,7 @@
       </c>
       <c r="J152"/>
     </row>
-    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>42</v>
       </c>
@@ -5496,7 +5490,7 @@
       </c>
       <c r="J162"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>42</v>
       </c>
@@ -5526,7 +5520,7 @@
       </c>
       <c r="J163"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>42</v>
       </c>
@@ -5556,7 +5550,7 @@
       </c>
       <c r="J164"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>42</v>
       </c>
@@ -5586,7 +5580,7 @@
       </c>
       <c r="J165"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>42</v>
       </c>
@@ -5616,7 +5610,7 @@
       </c>
       <c r="J166"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>42</v>
       </c>
@@ -5646,7 +5640,7 @@
       </c>
       <c r="J167"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>42</v>
       </c>
@@ -5695,14 +5689,14 @@
       <c r="F169" t="s">
         <v>24</v>
       </c>
-      <c r="G169">
-        <v>2715.9001117631901</v>
-      </c>
-      <c r="H169">
-        <v>162954.00670579099</v>
-      </c>
-      <c r="I169" s="5">
-        <v>1.0863600447052699</v>
+      <c r="G169" s="9">
+        <v>2677.35219330378</v>
+      </c>
+      <c r="H169" s="9">
+        <v>160641.131598226</v>
+      </c>
+      <c r="I169" s="9">
+        <v>1.0709408773215101</v>
       </c>
       <c r="J169"/>
     </row>
@@ -5725,14 +5719,14 @@
       <c r="F170" t="s">
         <v>22</v>
       </c>
-      <c r="G170">
-        <v>6362.0983551444197</v>
-      </c>
-      <c r="H170">
-        <v>381725.90130866499</v>
-      </c>
-      <c r="I170" s="5">
-        <v>2.54483934205776</v>
+      <c r="G170" s="9">
+        <v>6224.4272177893599</v>
+      </c>
+      <c r="H170" s="9">
+        <v>373465.63306736201</v>
+      </c>
+      <c r="I170" s="9">
+        <v>2.48977088711574</v>
       </c>
       <c r="J170"/>
     </row>
@@ -5755,13 +5749,13 @@
       <c r="F171" t="s">
         <v>26</v>
       </c>
-      <c r="G171">
+      <c r="G171" s="9">
         <v>27236.217376004999</v>
       </c>
-      <c r="H171">
+      <c r="H171" s="9">
         <v>1634173.0425603001</v>
       </c>
-      <c r="I171" s="5">
+      <c r="I171" s="9">
         <v>10.894486950401999</v>
       </c>
       <c r="J171"/>
@@ -5785,14 +5779,14 @@
       <c r="F172" t="s">
         <v>21</v>
       </c>
-      <c r="G172">
-        <v>4849.8216281485602</v>
-      </c>
-      <c r="H172">
-        <v>290989.29768891301</v>
-      </c>
-      <c r="I172" s="5">
-        <v>1.93992865125942</v>
+      <c r="G172" s="9">
+        <v>4780.9860594710399</v>
+      </c>
+      <c r="H172" s="9">
+        <v>286859.16356826201</v>
+      </c>
+      <c r="I172" s="9">
+        <v>1.9123944237884101</v>
       </c>
       <c r="J172"/>
     </row>
@@ -5815,14 +5809,14 @@
       <c r="F173" t="s">
         <v>25</v>
       </c>
-      <c r="G173">
-        <v>63144.677598494301</v>
-      </c>
-      <c r="H173">
-        <v>3788680.65590965</v>
-      </c>
-      <c r="I173" s="5">
-        <v>25.257871039397699</v>
+      <c r="G173" s="9">
+        <v>62248.438494312897</v>
+      </c>
+      <c r="H173" s="9">
+        <v>3734906.30965877</v>
+      </c>
+      <c r="I173" s="9">
+        <v>24.899375397725098</v>
       </c>
       <c r="J173"/>
     </row>
@@ -5845,13 +5839,13 @@
       <c r="F174" t="s">
         <v>23</v>
       </c>
-      <c r="G174">
+      <c r="G174" s="9">
         <v>29169.75</v>
       </c>
-      <c r="H174">
+      <c r="H174" s="9">
         <v>1750185</v>
       </c>
-      <c r="I174" s="5">
+      <c r="I174" s="9">
         <v>11.667899999999999</v>
       </c>
       <c r="J174"/>
@@ -5875,13 +5869,13 @@
       <c r="F175" t="s">
         <v>27</v>
       </c>
-      <c r="G175">
+      <c r="G175" s="9">
         <v>18172.713366666601</v>
       </c>
-      <c r="H175">
+      <c r="H175" s="9">
         <v>1090362.8019999999</v>
       </c>
-      <c r="I175" s="5">
+      <c r="I175" s="9">
         <v>7.2690853466666603</v>
       </c>
       <c r="J175"/>
@@ -5996,10 +5990,10 @@
         <v>18</v>
       </c>
       <c r="G179">
-        <v>22594.5166764401</v>
+        <v>11297.25833822005</v>
       </c>
       <c r="H179">
-        <v>632646.46694032406</v>
+        <v>316323.23347016203</v>
       </c>
       <c r="I179" s="5">
         <v>6.2762546323444903</v>
@@ -6186,7 +6180,7 @@
       </c>
       <c r="J185"/>
     </row>
-    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>43</v>
       </c>
@@ -6486,7 +6480,7 @@
       </c>
       <c r="J195"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>43</v>
       </c>
@@ -6516,7 +6510,7 @@
       </c>
       <c r="J196"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>43</v>
       </c>
@@ -6546,7 +6540,7 @@
       </c>
       <c r="J197"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>43</v>
       </c>
@@ -6576,7 +6570,7 @@
       </c>
       <c r="J198"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>43</v>
       </c>
@@ -6606,7 +6600,7 @@
       </c>
       <c r="J199"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>43</v>
       </c>
@@ -6636,7 +6630,7 @@
       </c>
       <c r="J200"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>43</v>
       </c>
@@ -6685,14 +6679,14 @@
       <c r="F202" t="s">
         <v>24</v>
       </c>
-      <c r="G202">
-        <v>4547.2666397718403</v>
-      </c>
-      <c r="H202">
-        <v>127323.465913611</v>
-      </c>
-      <c r="I202" s="5">
-        <v>1.2631296221588399</v>
+      <c r="G202" s="9">
+        <v>4484.0019930777999</v>
+      </c>
+      <c r="H202" s="9">
+        <v>125552.055806178</v>
+      </c>
+      <c r="I202" s="9">
+        <v>1.2455561091882801</v>
       </c>
       <c r="J202"/>
     </row>
@@ -6715,14 +6709,14 @@
       <c r="F203" t="s">
         <v>22</v>
       </c>
-      <c r="G203">
-        <v>12113.650811673901</v>
-      </c>
-      <c r="H203">
-        <v>339182.22272687103</v>
-      </c>
-      <c r="I203" s="5">
-        <v>3.36490300324277</v>
+      <c r="G203" s="9">
+        <v>11887.7056449095</v>
+      </c>
+      <c r="H203" s="9">
+        <v>332855.75805746799</v>
+      </c>
+      <c r="I203" s="9">
+        <v>3.3021404569193198</v>
       </c>
       <c r="J203"/>
     </row>
@@ -6745,13 +6739,13 @@
       <c r="F204" t="s">
         <v>26</v>
       </c>
-      <c r="G204">
+      <c r="G204" s="9">
         <v>55117.699983321399</v>
       </c>
-      <c r="H204">
+      <c r="H204" s="9">
         <v>1543295.59953299</v>
       </c>
-      <c r="I204" s="5">
+      <c r="I204" s="9">
         <v>15.310472217589201</v>
       </c>
       <c r="J204"/>
@@ -6775,14 +6769,14 @@
       <c r="F205" t="s">
         <v>21</v>
       </c>
-      <c r="G205">
-        <v>8120.1189995925697</v>
-      </c>
-      <c r="H205">
-        <v>227363.33198859199</v>
-      </c>
-      <c r="I205" s="5">
-        <v>2.25558861099793</v>
+      <c r="G205" s="9">
+        <v>8007.1464162103703</v>
+      </c>
+      <c r="H205" s="9">
+        <v>224200.09965389001</v>
+      </c>
+      <c r="I205" s="9">
+        <v>2.2242073378362099</v>
       </c>
       <c r="J205"/>
     </row>
@@ -6805,14 +6799,14 @@
       <c r="F206" t="s">
         <v>25</v>
       </c>
-      <c r="G206">
-        <v>105723.949374695</v>
-      </c>
-      <c r="H206">
-        <v>2960270.5824914598</v>
-      </c>
-      <c r="I206" s="5">
-        <v>29.367763715193099</v>
+      <c r="G206" s="9">
+        <v>104253.046339059</v>
+      </c>
+      <c r="H206" s="9">
+        <v>2919085.2974936501</v>
+      </c>
+      <c r="I206" s="9">
+        <v>28.959179538627499</v>
       </c>
       <c r="J206"/>
     </row>
@@ -6835,13 +6829,13 @@
       <c r="F207" t="s">
         <v>23</v>
       </c>
-      <c r="G207">
+      <c r="G207" s="9">
         <v>52491.1785714285</v>
       </c>
-      <c r="H207">
+      <c r="H207" s="9">
         <v>1469753</v>
       </c>
-      <c r="I207" s="5">
+      <c r="I207" s="9">
         <v>14.5808829365079</v>
       </c>
       <c r="J207"/>
@@ -6865,13 +6859,13 @@
       <c r="F208" t="s">
         <v>27</v>
       </c>
-      <c r="G208">
+      <c r="G208" s="9">
         <v>30052.964285714199</v>
       </c>
-      <c r="H208">
+      <c r="H208" s="9">
         <v>841483</v>
       </c>
-      <c r="I208" s="5">
+      <c r="I208" s="9">
         <v>8.3480456349206307</v>
       </c>
       <c r="J208"/>
@@ -6986,10 +6980,10 @@
         <v>18</v>
       </c>
       <c r="G212">
-        <v>34095.177724386704</v>
+        <v>17047.588862193352</v>
       </c>
       <c r="H212">
-        <v>954664.97628282697</v>
+        <v>477332.48814141349</v>
       </c>
       <c r="I212" s="5">
         <v>9.4708827012185299</v>
@@ -7172,7 +7166,7 @@
         <v>42.427747795912303</v>
       </c>
     </row>
-    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>44</v>
       </c>
@@ -7462,7 +7456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>44</v>
       </c>
@@ -7491,7 +7485,7 @@
         <v>4.4277152518070899</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>44</v>
       </c>
@@ -7520,7 +7514,7 @@
         <v>0.140997023809523</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>44</v>
       </c>
@@ -7549,7 +7543,7 @@
         <v>23.866980645429599</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>44</v>
       </c>
@@ -7578,7 +7572,7 @@
         <v>8.9217261904761909</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>44</v>
       </c>
@@ -7607,7 +7601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>44</v>
       </c>
@@ -7655,14 +7649,14 @@
       <c r="F235" t="s">
         <v>24</v>
       </c>
-      <c r="G235">
-        <v>5438.4071223926103</v>
-      </c>
-      <c r="H235">
-        <v>152275.39942699301</v>
-      </c>
-      <c r="I235" s="5">
-        <v>1.5106686451090601</v>
+      <c r="G235" s="9">
+        <v>5342.9406247643301</v>
+      </c>
+      <c r="H235" s="9">
+        <v>149602.33749340099</v>
+      </c>
+      <c r="I235" s="9">
+        <v>1.4841501735456399</v>
       </c>
     </row>
     <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -7684,14 +7678,14 @@
       <c r="F236" t="s">
         <v>22</v>
       </c>
-      <c r="G236">
-        <v>14643.796242222201</v>
-      </c>
-      <c r="H236">
-        <v>410026.29478222202</v>
-      </c>
-      <c r="I236" s="5">
-        <v>4.0677211783950602</v>
+      <c r="G236" s="9">
+        <v>14302.8444649783</v>
+      </c>
+      <c r="H236" s="9">
+        <v>400479.64501939301</v>
+      </c>
+      <c r="I236" s="9">
+        <v>3.9730123513828701</v>
       </c>
     </row>
     <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -7713,13 +7707,13 @@
       <c r="F237" t="s">
         <v>26</v>
       </c>
-      <c r="G237">
+      <c r="G237" s="9">
         <v>55117.699983321399</v>
       </c>
-      <c r="H237">
+      <c r="H237" s="9">
         <v>1543295.59953299</v>
       </c>
-      <c r="I237" s="5">
+      <c r="I237" s="9">
         <v>15.310472217589201</v>
       </c>
     </row>
@@ -7742,14 +7736,14 @@
       <c r="F238" t="s">
         <v>21</v>
       </c>
-      <c r="G238">
-        <v>9711.4412899868094</v>
-      </c>
-      <c r="H238">
-        <v>271920.35611962999</v>
-      </c>
-      <c r="I238" s="5">
-        <v>2.6976225805518901</v>
+      <c r="G238" s="9">
+        <v>9540.9654013648797</v>
+      </c>
+      <c r="H238" s="9">
+        <v>267147.03123821598</v>
+      </c>
+      <c r="I238" s="9">
+        <v>2.6502681670457999</v>
       </c>
     </row>
     <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -7771,14 +7765,14 @@
       <c r="F239" t="s">
         <v>25</v>
       </c>
-      <c r="G239">
-        <v>126442.965595628</v>
-      </c>
-      <c r="H239">
-        <v>3540403.0366775901</v>
-      </c>
-      <c r="I239" s="5">
-        <v>35.123045998785599</v>
+      <c r="G239" s="9">
+        <v>124223.36952577</v>
+      </c>
+      <c r="H239" s="9">
+        <v>3478254.3467215798</v>
+      </c>
+      <c r="I239" s="9">
+        <v>34.506491534936302</v>
       </c>
     </row>
     <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -7800,13 +7794,13 @@
       <c r="F240" t="s">
         <v>23</v>
       </c>
-      <c r="G240">
+      <c r="G240" s="9">
         <v>60048.321428571398</v>
       </c>
-      <c r="H240">
+      <c r="H240" s="9">
         <v>1681353</v>
       </c>
-      <c r="I240" s="5">
+      <c r="I240" s="9">
         <v>16.6800892857142</v>
       </c>
     </row>
@@ -7829,13 +7823,13 @@
       <c r="F241" t="s">
         <v>27</v>
       </c>
-      <c r="G241">
+      <c r="G241" s="9">
         <v>30052.964285714199</v>
       </c>
-      <c r="H241">
+      <c r="H241" s="9">
         <v>841483</v>
       </c>
-      <c r="I241" s="5">
+      <c r="I241" s="9">
         <v>8.3480456349206307</v>
       </c>
     </row>
@@ -7843,7 +7837,7 @@
   <autoFilter ref="A1:I241" xr:uid="{74B3986E-2BCE-704E-B480-617FD308BB93}">
     <filterColumn colId="3">
       <filters>
-        <filter val="ErectionCost"/>
+        <filter val="GridConnectionCost"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>